<commit_message>
config building required resources.
</commit_message>
<xml_diff>
--- a/Unity/Assets/Config/Excel/MicroDustBuildingConfig.xlsx
+++ b/Unity/Assets/Config/Excel/MicroDustBuildingConfig.xlsx
@@ -7,7 +7,7 @@
     <workbookView windowWidth="28800" windowHeight="13670"/>
   </bookViews>
   <sheets>
-    <sheet name="UnitProto" sheetId="1" r:id="rId1"/>
+    <sheet name="Buildings" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="51">
   <si>
     <t>Id</t>
   </si>
@@ -50,25 +50,37 @@
     <t>MaxLevel</t>
   </si>
   <si>
+    <t>Stone</t>
+  </si>
+  <si>
+    <t>Wood</t>
+  </si>
+  <si>
+    <t>Metal</t>
+  </si>
+  <si>
     <t>int</t>
   </si>
   <si>
     <t>string</t>
   </si>
   <si>
+    <t>int[]</t>
+  </si>
+  <si>
     <t>Storage</t>
   </si>
   <si>
+    <t>20,20,20</t>
+  </si>
+  <si>
+    <t>20,30,20</t>
+  </si>
+  <si>
+    <t>20,10</t>
+  </si>
+  <si>
     <t>Food</t>
-  </si>
-  <si>
-    <t>Stone</t>
-  </si>
-  <si>
-    <t>Wood</t>
-  </si>
-  <si>
-    <t>Metal</t>
   </si>
   <si>
     <t>Gold</t>
@@ -807,15 +819,12 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1174,10 +1183,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="C3:I49"/>
+  <dimension ref="C3:L49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G48" sqref="G48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13"/>
@@ -1185,93 +1194,116 @@
     <col min="1" max="1" width="21.1272727272727" style="2" customWidth="1"/>
     <col min="2" max="2" width="12.7545454545455" style="2" customWidth="1"/>
     <col min="3" max="4" width="12.6272727272727" style="2" customWidth="1"/>
-    <col min="5" max="5" width="24" style="3" customWidth="1"/>
-    <col min="6" max="6" width="12.1818181818182" style="3" customWidth="1"/>
+    <col min="5" max="5" width="24" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1818181818182" style="1" customWidth="1"/>
     <col min="7" max="7" width="25.3636363636364" style="2" customWidth="1"/>
     <col min="8" max="8" width="12.6272727272727" style="2" customWidth="1"/>
-    <col min="9" max="9" width="12.6272727272727" style="3" customWidth="1"/>
-    <col min="10" max="10" width="15.5454545454545" style="2" customWidth="1"/>
-    <col min="11" max="11" width="12.6363636363636" style="2" customWidth="1"/>
-    <col min="12" max="12" width="14.7272727272727" style="2" customWidth="1"/>
-    <col min="13" max="13" width="15.7272727272727" style="2" customWidth="1"/>
-    <col min="14" max="14" width="13.5454545454545" style="2" customWidth="1"/>
-    <col min="15" max="15" width="12.6363636363636" style="2" customWidth="1"/>
-    <col min="16" max="16" width="14.7272727272727" style="2" customWidth="1"/>
-    <col min="17" max="17" width="15.7272727272727" style="2" customWidth="1"/>
-    <col min="18" max="18" width="13.5454545454545" style="2" customWidth="1"/>
-    <col min="19" max="16384" width="9" style="2"/>
+    <col min="9" max="12" width="12.6272727272727" style="1" customWidth="1"/>
+    <col min="13" max="13" width="13.5454545454545" style="2" customWidth="1"/>
+    <col min="14" max="14" width="12.6363636363636" style="2" customWidth="1"/>
+    <col min="15" max="15" width="14.7272727272727" style="2" customWidth="1"/>
+    <col min="16" max="16" width="15.7272727272727" style="2" customWidth="1"/>
+    <col min="17" max="17" width="13.5454545454545" style="2" customWidth="1"/>
+    <col min="18" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="3" ht="13.5" spans="3:9">
-      <c r="C3" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="4" t="s">
+    <row r="3" ht="13.5" spans="3:12">
+      <c r="C3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="I3" s="5" t="s">
+      <c r="H3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" ht="13.5" spans="3:9">
-      <c r="C4" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4" s="4" t="s">
+      <c r="J3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" ht="13.5" spans="3:12">
+      <c r="C4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="I4" s="5" t="s">
+      <c r="H4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" ht="13.5" spans="3:9">
-      <c r="C5" s="4" t="s">
+      <c r="J4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" s="4" t="s">
+      <c r="K4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" s="1" customFormat="1" spans="3:9">
+      <c r="L4" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" ht="13.5" spans="3:12">
+      <c r="C5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" s="1" customFormat="1" spans="3:12">
       <c r="C6" s="1">
         <v>1001</v>
       </c>
@@ -1281,11 +1313,11 @@
       <c r="E6" s="1">
         <v>1</v>
       </c>
-      <c r="F6" s="6">
-        <v>2</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>9</v>
+      <c r="F6" s="5">
+        <v>2</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="H6" s="1">
         <v>0</v>
@@ -1293,8 +1325,17 @@
       <c r="I6" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" s="1" customFormat="1" ht="15" customHeight="1" spans="3:9">
+      <c r="J6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" s="1" customFormat="1" ht="15" customHeight="1" spans="3:12">
       <c r="C7" s="1">
         <v>1002</v>
       </c>
@@ -1304,11 +1345,11 @@
       <c r="E7" s="1">
         <v>2</v>
       </c>
-      <c r="F7" s="6">
-        <v>2</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>10</v>
+      <c r="F7" s="5">
+        <v>2</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="H7" s="1">
         <v>0</v>
@@ -1316,8 +1357,17 @@
       <c r="I7" s="1">
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="3:9">
+      <c r="J7" s="1">
+        <v>30</v>
+      </c>
+      <c r="K7" s="1">
+        <v>30</v>
+      </c>
+      <c r="L7" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="3:12">
       <c r="C8" s="1">
         <v>1003</v>
       </c>
@@ -1327,11 +1377,11 @@
       <c r="E8" s="1">
         <v>2</v>
       </c>
-      <c r="F8" s="6">
-        <v>3</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>11</v>
+      <c r="F8" s="5">
+        <v>3</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="H8" s="1">
         <v>0</v>
@@ -1339,8 +1389,17 @@
       <c r="I8" s="1">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="3:9">
+      <c r="J8" s="1">
+        <v>30</v>
+      </c>
+      <c r="K8" s="1">
+        <v>30</v>
+      </c>
+      <c r="L8" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="3:12">
       <c r="C9" s="1">
         <v>1004</v>
       </c>
@@ -1350,11 +1409,11 @@
       <c r="E9" s="1">
         <v>3</v>
       </c>
-      <c r="F9" s="6">
-        <v>2</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>12</v>
+      <c r="F9" s="5">
+        <v>2</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="H9" s="1">
         <v>0</v>
@@ -1362,8 +1421,17 @@
       <c r="I9" s="1">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" spans="3:9">
+      <c r="J9" s="1">
+        <v>30</v>
+      </c>
+      <c r="K9" s="1">
+        <v>30</v>
+      </c>
+      <c r="L9" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="3:12">
       <c r="C10" s="1">
         <v>1005</v>
       </c>
@@ -1373,11 +1441,11 @@
       <c r="E10" s="1">
         <v>3</v>
       </c>
-      <c r="F10" s="6">
-        <v>3</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>13</v>
+      <c r="F10" s="5">
+        <v>3</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="H10" s="1">
         <v>0</v>
@@ -1385,8 +1453,17 @@
       <c r="I10" s="1">
         <v>30</v>
       </c>
-    </row>
-    <row r="11" spans="3:9">
+      <c r="J10" s="1">
+        <v>30</v>
+      </c>
+      <c r="K10" s="1">
+        <v>30</v>
+      </c>
+      <c r="L10" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="3:12">
       <c r="C11" s="1">
         <v>1006</v>
       </c>
@@ -1396,11 +1473,11 @@
       <c r="E11" s="1">
         <v>4</v>
       </c>
-      <c r="F11" s="6">
-        <v>1</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>14</v>
+      <c r="F11" s="5">
+        <v>1</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="H11" s="1">
         <v>0</v>
@@ -1408,8 +1485,17 @@
       <c r="I11" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="3:9">
+      <c r="J11" s="1">
+        <v>20</v>
+      </c>
+      <c r="K11" s="1">
+        <v>20</v>
+      </c>
+      <c r="L11" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="3:12">
       <c r="C12" s="1">
         <v>1007</v>
       </c>
@@ -1419,11 +1505,11 @@
       <c r="E12" s="1">
         <v>5</v>
       </c>
-      <c r="F12" s="6">
-        <v>1</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>15</v>
+      <c r="F12" s="5">
+        <v>1</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="H12" s="1">
         <v>0</v>
@@ -1431,8 +1517,17 @@
       <c r="I12" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="3:9">
+      <c r="J12" s="1">
+        <v>3</v>
+      </c>
+      <c r="K12" s="1">
+        <v>3</v>
+      </c>
+      <c r="L12" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="3:12">
       <c r="C13" s="1">
         <v>1008</v>
       </c>
@@ -1442,11 +1537,11 @@
       <c r="E13" s="1">
         <v>6</v>
       </c>
-      <c r="F13" s="6">
-        <v>3</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>16</v>
+      <c r="F13" s="5">
+        <v>3</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="H13" s="1">
         <v>0</v>
@@ -1454,8 +1549,17 @@
       <c r="I13" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="3:9">
+      <c r="J13" s="1">
+        <v>4</v>
+      </c>
+      <c r="K13" s="1">
+        <v>4</v>
+      </c>
+      <c r="L13" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="3:12">
       <c r="C14" s="1">
         <v>1009</v>
       </c>
@@ -1465,11 +1569,11 @@
       <c r="E14" s="1">
         <v>7</v>
       </c>
-      <c r="F14" s="6">
-        <v>1</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>17</v>
+      <c r="F14" s="5">
+        <v>1</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="H14" s="1">
         <v>0</v>
@@ -1477,8 +1581,17 @@
       <c r="I14" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="3:9">
+      <c r="J14" s="1">
+        <v>5</v>
+      </c>
+      <c r="K14" s="1">
+        <v>5</v>
+      </c>
+      <c r="L14" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="3:12">
       <c r="C15" s="1">
         <v>1010</v>
       </c>
@@ -1488,11 +1601,11 @@
       <c r="E15" s="1">
         <v>8</v>
       </c>
-      <c r="F15" s="6">
-        <v>2</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>18</v>
+      <c r="F15" s="5">
+        <v>2</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="H15" s="1">
         <v>0</v>
@@ -1500,8 +1613,17 @@
       <c r="I15" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="3:9">
+      <c r="J15" s="1">
+        <v>5</v>
+      </c>
+      <c r="K15" s="1">
+        <v>5</v>
+      </c>
+      <c r="L15" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="3:12">
       <c r="C16" s="1">
         <v>1011</v>
       </c>
@@ -1511,11 +1633,11 @@
       <c r="E16" s="1">
         <v>9</v>
       </c>
-      <c r="F16" s="6">
-        <v>3</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>19</v>
+      <c r="F16" s="5">
+        <v>3</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="H16" s="1">
         <v>0</v>
@@ -1523,8 +1645,17 @@
       <c r="I16" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="3:9">
+      <c r="J16" s="1">
+        <v>4</v>
+      </c>
+      <c r="K16" s="1">
+        <v>4</v>
+      </c>
+      <c r="L16" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="3:12">
       <c r="C17" s="1">
         <v>1012</v>
       </c>
@@ -1534,11 +1665,11 @@
       <c r="E17" s="1">
         <v>10</v>
       </c>
-      <c r="F17" s="6">
-        <v>2</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>20</v>
+      <c r="F17" s="5">
+        <v>2</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="H17" s="1">
         <v>0</v>
@@ -1546,8 +1677,17 @@
       <c r="I17" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="3:9">
+      <c r="J17" s="1">
+        <v>5</v>
+      </c>
+      <c r="K17" s="1">
+        <v>5</v>
+      </c>
+      <c r="L17" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="3:12">
       <c r="C18" s="1">
         <v>1013</v>
       </c>
@@ -1557,11 +1697,11 @@
       <c r="E18" s="1">
         <v>1</v>
       </c>
-      <c r="F18" s="6">
-        <v>1</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>21</v>
+      <c r="F18" s="5">
+        <v>1</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="H18" s="1">
         <v>0</v>
@@ -1569,8 +1709,17 @@
       <c r="I18" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="3:9">
+      <c r="J18" s="1">
+        <v>5</v>
+      </c>
+      <c r="K18" s="1">
+        <v>5</v>
+      </c>
+      <c r="L18" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="3:12">
       <c r="C19" s="1">
         <v>1014</v>
       </c>
@@ -1580,11 +1729,11 @@
       <c r="E19" s="1">
         <v>2</v>
       </c>
-      <c r="F19" s="6">
-        <v>2</v>
-      </c>
-      <c r="G19" s="7" t="s">
-        <v>22</v>
+      <c r="F19" s="5">
+        <v>2</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="H19" s="1">
         <v>0</v>
@@ -1592,8 +1741,17 @@
       <c r="I19" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="20" spans="3:9">
+      <c r="J19" s="1">
+        <v>10</v>
+      </c>
+      <c r="K19" s="1">
+        <v>10</v>
+      </c>
+      <c r="L19" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="3:12">
       <c r="C20" s="1">
         <v>1015</v>
       </c>
@@ -1603,11 +1761,11 @@
       <c r="E20" s="1">
         <v>2</v>
       </c>
-      <c r="F20" s="6">
-        <v>3</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>23</v>
+      <c r="F20" s="5">
+        <v>3</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>27</v>
       </c>
       <c r="H20" s="1">
         <v>0</v>
@@ -1615,22 +1773,31 @@
       <c r="I20" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="21" spans="3:9">
+      <c r="J20" s="1">
+        <v>10</v>
+      </c>
+      <c r="K20" s="1">
+        <v>10</v>
+      </c>
+      <c r="L20" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="3:12">
       <c r="C21" s="1">
         <v>1016</v>
       </c>
       <c r="D21" s="1">
         <v>2</v>
       </c>
-      <c r="E21" s="3">
-        <v>3</v>
-      </c>
-      <c r="F21" s="3">
+      <c r="E21" s="1">
+        <v>3</v>
+      </c>
+      <c r="F21" s="1">
         <v>1</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="H21" s="1">
         <v>0</v>
@@ -1638,22 +1805,31 @@
       <c r="I21" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="22" spans="3:9">
+      <c r="J21" s="1">
+        <v>10</v>
+      </c>
+      <c r="K21" s="1">
+        <v>10</v>
+      </c>
+      <c r="L21" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="3:12">
       <c r="C22" s="1">
         <v>1017</v>
       </c>
       <c r="D22" s="1">
         <v>2</v>
       </c>
-      <c r="E22" s="3">
-        <v>3</v>
-      </c>
-      <c r="F22" s="3">
+      <c r="E22" s="1">
+        <v>3</v>
+      </c>
+      <c r="F22" s="1">
         <v>2</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="H22" s="1">
         <v>0</v>
@@ -1661,22 +1837,31 @@
       <c r="I22" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="23" spans="3:9">
+      <c r="J22" s="1">
+        <v>10</v>
+      </c>
+      <c r="K22" s="1">
+        <v>10</v>
+      </c>
+      <c r="L22" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="3:12">
       <c r="C23" s="1">
         <v>1018</v>
       </c>
       <c r="D23" s="1">
         <v>2</v>
       </c>
-      <c r="E23" s="3">
-        <v>3</v>
-      </c>
-      <c r="F23" s="3">
+      <c r="E23" s="1">
+        <v>3</v>
+      </c>
+      <c r="F23" s="1">
         <v>3</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="H23" s="1">
         <v>0</v>
@@ -1684,510 +1869,717 @@
       <c r="I23" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="24" spans="3:9">
+      <c r="J23" s="1">
+        <v>10</v>
+      </c>
+      <c r="K23" s="1">
+        <v>10</v>
+      </c>
+      <c r="L23" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="3:12">
       <c r="C24" s="1">
         <v>1019</v>
       </c>
       <c r="D24" s="1">
         <v>2</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E24" s="1">
         <v>4</v>
       </c>
-      <c r="F24" s="3">
+      <c r="F24" s="1">
         <v>1</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="H24" s="1">
         <v>0</v>
       </c>
-      <c r="I24" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="3:9">
+      <c r="I24" s="1">
+        <v>5</v>
+      </c>
+      <c r="J24" s="1">
+        <v>5</v>
+      </c>
+      <c r="K24" s="1">
+        <v>5</v>
+      </c>
+      <c r="L24" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="3:12">
       <c r="C25" s="1">
         <v>1020</v>
       </c>
       <c r="D25" s="1">
         <v>2</v>
       </c>
-      <c r="E25" s="3">
-        <v>5</v>
-      </c>
-      <c r="F25" s="3">
+      <c r="E25" s="1">
+        <v>5</v>
+      </c>
+      <c r="F25" s="1">
         <v>1</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="H25" s="1">
         <v>0</v>
       </c>
-      <c r="I25" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="3:9">
+      <c r="I25" s="1">
+        <v>10</v>
+      </c>
+      <c r="J25" s="1">
+        <v>10</v>
+      </c>
+      <c r="K25" s="1">
+        <v>10</v>
+      </c>
+      <c r="L25" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="3:12">
       <c r="C26" s="1">
         <v>1021</v>
       </c>
       <c r="D26" s="1">
         <v>2</v>
       </c>
-      <c r="E26" s="3">
-        <v>5</v>
-      </c>
-      <c r="F26" s="3">
+      <c r="E26" s="1">
+        <v>5</v>
+      </c>
+      <c r="F26" s="1">
         <v>2</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H26" s="1">
         <v>0</v>
       </c>
-      <c r="I26" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="3:9">
+      <c r="I26" s="1">
+        <v>10</v>
+      </c>
+      <c r="J26" s="1">
+        <v>10</v>
+      </c>
+      <c r="K26" s="1">
+        <v>10</v>
+      </c>
+      <c r="L26" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="3:12">
       <c r="C27" s="1">
         <v>1022</v>
       </c>
       <c r="D27" s="1">
         <v>2</v>
       </c>
-      <c r="E27" s="3">
-        <v>5</v>
-      </c>
-      <c r="F27" s="3">
+      <c r="E27" s="1">
+        <v>5</v>
+      </c>
+      <c r="F27" s="1">
         <v>3</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="H27" s="1">
         <v>0</v>
       </c>
-      <c r="I27" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="3:9">
+      <c r="I27" s="1">
+        <v>10</v>
+      </c>
+      <c r="J27" s="1">
+        <v>10</v>
+      </c>
+      <c r="K27" s="1">
+        <v>10</v>
+      </c>
+      <c r="L27" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="3:12">
       <c r="C28" s="1">
         <v>1023</v>
       </c>
       <c r="D28" s="1">
         <v>2</v>
       </c>
-      <c r="E28" s="3">
+      <c r="E28" s="1">
         <v>6</v>
       </c>
-      <c r="F28" s="3">
+      <c r="F28" s="1">
         <v>1</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="H28" s="1">
         <v>0</v>
       </c>
-      <c r="I28" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="3:9">
+      <c r="I28" s="1">
+        <v>10</v>
+      </c>
+      <c r="J28" s="1">
+        <v>10</v>
+      </c>
+      <c r="K28" s="1">
+        <v>10</v>
+      </c>
+      <c r="L28" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="3:12">
       <c r="C29" s="1">
         <v>1024</v>
       </c>
       <c r="D29" s="1">
         <v>2</v>
       </c>
-      <c r="E29" s="3">
+      <c r="E29" s="1">
         <v>7</v>
       </c>
-      <c r="F29" s="3">
+      <c r="F29" s="1">
         <v>3</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="H29" s="1">
         <v>0</v>
       </c>
-      <c r="I29" s="3">
+      <c r="I29" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="30" spans="3:9">
+      <c r="J29" s="1">
+        <v>20</v>
+      </c>
+      <c r="K29" s="1">
+        <v>20</v>
+      </c>
+      <c r="L29" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="3:12">
       <c r="C30" s="1">
         <v>1025</v>
       </c>
       <c r="D30" s="1">
         <v>2</v>
       </c>
-      <c r="E30" s="3">
+      <c r="E30" s="1">
         <v>8</v>
       </c>
-      <c r="F30" s="3">
+      <c r="F30" s="1">
         <v>3</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="H30" s="1">
         <v>0</v>
       </c>
-      <c r="I30" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="3:9">
+      <c r="I30" s="1">
+        <v>3</v>
+      </c>
+      <c r="J30" s="1">
+        <v>3</v>
+      </c>
+      <c r="K30" s="1">
+        <v>3</v>
+      </c>
+      <c r="L30" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="3:12">
       <c r="C31" s="1">
         <v>1026</v>
       </c>
       <c r="D31" s="1">
         <v>2</v>
       </c>
-      <c r="E31" s="3">
+      <c r="E31" s="1">
         <v>9</v>
       </c>
-      <c r="F31" s="3">
+      <c r="F31" s="1">
         <v>1</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="H31" s="1">
         <v>0</v>
       </c>
-      <c r="I31" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="32" spans="3:9">
+      <c r="I31" s="1">
+        <v>10</v>
+      </c>
+      <c r="J31" s="1">
+        <v>10</v>
+      </c>
+      <c r="K31" s="1">
+        <v>10</v>
+      </c>
+      <c r="L31" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="3:12">
       <c r="C32" s="1">
         <v>1027</v>
       </c>
       <c r="D32" s="1">
         <v>2</v>
       </c>
-      <c r="E32" s="3">
+      <c r="E32" s="1">
         <v>9</v>
       </c>
-      <c r="F32" s="3">
+      <c r="F32" s="1">
         <v>2</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="H32" s="1">
         <v>0</v>
       </c>
-      <c r="I32" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" spans="3:9">
+      <c r="I32" s="1">
+        <v>10</v>
+      </c>
+      <c r="J32" s="1">
+        <v>10</v>
+      </c>
+      <c r="K32" s="1">
+        <v>10</v>
+      </c>
+      <c r="L32" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="3:12">
       <c r="C33" s="1">
         <v>1028</v>
       </c>
       <c r="D33" s="1">
         <v>2</v>
       </c>
-      <c r="E33" s="3">
-        <v>10</v>
-      </c>
-      <c r="F33" s="3">
+      <c r="E33" s="1">
+        <v>10</v>
+      </c>
+      <c r="F33" s="1">
         <v>1</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="H33" s="1">
         <v>0</v>
       </c>
-      <c r="I33" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="34" spans="3:9">
+      <c r="I33" s="1">
+        <v>10</v>
+      </c>
+      <c r="J33" s="1">
+        <v>10</v>
+      </c>
+      <c r="K33" s="1">
+        <v>10</v>
+      </c>
+      <c r="L33" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="3:12">
       <c r="C34" s="1">
         <v>1029</v>
       </c>
       <c r="D34" s="1">
         <v>2</v>
       </c>
-      <c r="E34" s="3">
-        <v>10</v>
-      </c>
-      <c r="F34" s="3">
+      <c r="E34" s="1">
+        <v>10</v>
+      </c>
+      <c r="F34" s="1">
         <v>2</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="H34" s="1">
         <v>0</v>
       </c>
-      <c r="I34" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="35" spans="3:9">
+      <c r="I34" s="1">
+        <v>10</v>
+      </c>
+      <c r="J34" s="1">
+        <v>10</v>
+      </c>
+      <c r="K34" s="1">
+        <v>10</v>
+      </c>
+      <c r="L34" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="3:12">
       <c r="C35" s="1">
         <v>1030</v>
       </c>
       <c r="D35" s="1">
         <v>2</v>
       </c>
-      <c r="E35" s="3">
-        <v>10</v>
-      </c>
-      <c r="F35" s="3">
+      <c r="E35" s="1">
+        <v>10</v>
+      </c>
+      <c r="F35" s="1">
         <v>3</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="H35" s="1">
         <v>0</v>
       </c>
-      <c r="I35" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="36" spans="3:9">
+      <c r="I35" s="1">
+        <v>10</v>
+      </c>
+      <c r="J35" s="1">
+        <v>10</v>
+      </c>
+      <c r="K35" s="1">
+        <v>10</v>
+      </c>
+      <c r="L35" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="3:12">
       <c r="C36" s="1">
         <v>1031</v>
       </c>
       <c r="D36" s="1">
         <v>3</v>
       </c>
-      <c r="E36" s="3">
+      <c r="E36" s="1">
         <v>4</v>
       </c>
-      <c r="F36" s="3">
+      <c r="F36" s="1">
         <v>1</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="H36" s="1">
         <v>0</v>
       </c>
-      <c r="I36" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="37" spans="3:9">
+      <c r="I36" s="1">
+        <v>5</v>
+      </c>
+      <c r="J36" s="1">
+        <v>5</v>
+      </c>
+      <c r="K36" s="1">
+        <v>5</v>
+      </c>
+      <c r="L36" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="3:12">
       <c r="C37" s="1">
         <v>1032</v>
       </c>
       <c r="D37" s="1">
         <v>3</v>
       </c>
-      <c r="E37" s="3">
+      <c r="E37" s="1">
         <v>4</v>
       </c>
-      <c r="F37" s="3">
+      <c r="F37" s="1">
         <v>3</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="H37" s="1">
         <v>0</v>
       </c>
-      <c r="I37" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38" spans="3:9">
+      <c r="I37" s="1">
+        <v>5</v>
+      </c>
+      <c r="J37" s="1">
+        <v>5</v>
+      </c>
+      <c r="K37" s="1">
+        <v>5</v>
+      </c>
+      <c r="L37" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="3:12">
       <c r="C38" s="1">
         <v>1033</v>
       </c>
       <c r="D38" s="1">
         <v>3</v>
       </c>
-      <c r="E38" s="3">
-        <v>5</v>
-      </c>
-      <c r="F38" s="3">
+      <c r="E38" s="1">
+        <v>5</v>
+      </c>
+      <c r="F38" s="1">
         <v>2</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="H38" s="1">
         <v>0</v>
       </c>
-      <c r="I38" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="39" spans="3:9">
+      <c r="I38" s="1">
+        <v>10</v>
+      </c>
+      <c r="J38" s="1">
+        <v>10</v>
+      </c>
+      <c r="K38" s="1">
+        <v>10</v>
+      </c>
+      <c r="L38" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="3:12">
       <c r="C39" s="1">
         <v>1034</v>
       </c>
       <c r="D39" s="1">
         <v>3</v>
       </c>
-      <c r="E39" s="3">
+      <c r="E39" s="1">
         <v>6</v>
       </c>
-      <c r="F39" s="3">
+      <c r="F39" s="1">
         <v>3</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="H39" s="1">
         <v>0</v>
       </c>
-      <c r="I39" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="3:9">
+      <c r="I39" s="1">
+        <v>3</v>
+      </c>
+      <c r="J39" s="1">
+        <v>3</v>
+      </c>
+      <c r="K39" s="1">
+        <v>3</v>
+      </c>
+      <c r="L39" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="3:12">
       <c r="C40" s="1">
         <v>1035</v>
       </c>
       <c r="D40" s="1">
         <v>3</v>
       </c>
-      <c r="E40" s="3">
+      <c r="E40" s="1">
         <v>7</v>
       </c>
-      <c r="F40" s="3">
+      <c r="F40" s="1">
         <v>2</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="H40" s="1">
         <v>0</v>
       </c>
-      <c r="I40" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="41" spans="3:9">
+      <c r="I40" s="1">
+        <v>10</v>
+      </c>
+      <c r="J40" s="1">
+        <v>10</v>
+      </c>
+      <c r="K40" s="1">
+        <v>10</v>
+      </c>
+      <c r="L40" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="3:12">
       <c r="C41" s="1">
         <v>1036</v>
       </c>
       <c r="D41" s="1">
         <v>3</v>
       </c>
-      <c r="E41" s="3">
+      <c r="E41" s="1">
         <v>8</v>
       </c>
-      <c r="F41" s="3">
+      <c r="F41" s="1">
         <v>1</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="H41" s="1">
         <v>0</v>
       </c>
-      <c r="I41" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="42" spans="3:9">
+      <c r="I41" s="1">
+        <v>5</v>
+      </c>
+      <c r="J41" s="1">
+        <v>5</v>
+      </c>
+      <c r="K41" s="1">
+        <v>5</v>
+      </c>
+      <c r="L41" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="3:12">
       <c r="C42" s="1">
         <v>1037</v>
       </c>
       <c r="D42" s="1">
         <v>3</v>
       </c>
-      <c r="E42" s="3">
+      <c r="E42" s="1">
         <v>8</v>
       </c>
-      <c r="F42" s="3">
+      <c r="F42" s="1">
         <v>2</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="H42" s="1">
         <v>0</v>
       </c>
-      <c r="I42" s="3">
+      <c r="I42" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="43" spans="3:9">
+      <c r="J42" s="1">
+        <v>4</v>
+      </c>
+      <c r="K42" s="1">
+        <v>4</v>
+      </c>
+      <c r="L42" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="3:12">
       <c r="C43" s="1">
         <v>1038</v>
       </c>
       <c r="D43" s="1">
         <v>3</v>
       </c>
-      <c r="E43" s="3">
+      <c r="E43" s="1">
         <v>9</v>
       </c>
-      <c r="F43" s="3">
+      <c r="F43" s="1">
         <v>1</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="H43" s="1">
         <v>0</v>
       </c>
-      <c r="I43" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="44" spans="3:9">
+      <c r="I43" s="1">
+        <v>5</v>
+      </c>
+      <c r="J43" s="1">
+        <v>5</v>
+      </c>
+      <c r="K43" s="1">
+        <v>5</v>
+      </c>
+      <c r="L43" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="3:12">
       <c r="C44" s="1">
         <v>1039</v>
       </c>
       <c r="D44" s="1">
         <v>3</v>
       </c>
-      <c r="E44" s="3">
+      <c r="E44" s="1">
         <v>9</v>
       </c>
-      <c r="F44" s="3">
+      <c r="F44" s="1">
         <v>3</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="H44" s="1">
         <v>0</v>
       </c>
-      <c r="I44" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="45" spans="3:9">
+      <c r="I44" s="1">
+        <v>5</v>
+      </c>
+      <c r="J44" s="1">
+        <v>5</v>
+      </c>
+      <c r="K44" s="1">
+        <v>5</v>
+      </c>
+      <c r="L44" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="3:12">
       <c r="C45" s="1">
         <v>1040</v>
       </c>
       <c r="D45" s="1">
         <v>3</v>
       </c>
-      <c r="E45" s="3">
-        <v>10</v>
-      </c>
-      <c r="F45" s="3">
+      <c r="E45" s="1">
+        <v>10</v>
+      </c>
+      <c r="F45" s="1">
         <v>2</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="H45" s="1">
         <v>0</v>
       </c>
-      <c r="I45" s="3">
+      <c r="I45" s="1">
+        <v>5</v>
+      </c>
+      <c r="J45" s="1">
+        <v>5</v>
+      </c>
+      <c r="K45" s="1">
+        <v>5</v>
+      </c>
+      <c r="L45" s="1">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
upgrade to unity 6
</commit_message>
<xml_diff>
--- a/Unity/Assets/Config/Excel/MicroDustBuildingConfig.xlsx
+++ b/Unity/Assets/Config/Excel/MicroDustBuildingConfig.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="53">
   <si>
     <t>Id</t>
   </si>
@@ -59,6 +59,9 @@
     <t>Metal</t>
   </si>
   <si>
+    <t>Description</t>
+  </si>
+  <si>
     <t>int</t>
   </si>
   <si>
@@ -78,6 +81,9 @@
   </si>
   <si>
     <t>20,10</t>
+  </si>
+  <si>
+    <t>Storage + 100</t>
   </si>
   <si>
     <t>Food</t>
@@ -1183,10 +1189,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="C3:L49"/>
+  <dimension ref="C3:M49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="N35" sqref="N35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13"/>
@@ -1198,8 +1204,7 @@
     <col min="6" max="6" width="12.1818181818182" style="1" customWidth="1"/>
     <col min="7" max="7" width="25.3636363636364" style="2" customWidth="1"/>
     <col min="8" max="8" width="12.6272727272727" style="2" customWidth="1"/>
-    <col min="9" max="12" width="12.6272727272727" style="1" customWidth="1"/>
-    <col min="13" max="13" width="13.5454545454545" style="2" customWidth="1"/>
+    <col min="9" max="13" width="12.6272727272727" style="1" customWidth="1"/>
     <col min="14" max="14" width="12.6363636363636" style="2" customWidth="1"/>
     <col min="15" max="15" width="14.7272727272727" style="2" customWidth="1"/>
     <col min="16" max="16" width="15.7272727272727" style="2" customWidth="1"/>
@@ -1207,7 +1212,7 @@
     <col min="18" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="3" ht="13.5" spans="3:12">
+    <row r="3" ht="13.5" spans="3:13">
       <c r="C3" s="3" t="s">
         <v>0</v>
       </c>
@@ -1238,8 +1243,11 @@
       <c r="L3" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" ht="13.5" spans="3:12">
+      <c r="M3" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" ht="13.5" spans="3:13">
       <c r="C4" s="3" t="s">
         <v>0</v>
       </c>
@@ -1270,40 +1278,46 @@
       <c r="L4" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" ht="13.5" spans="3:12">
+      <c r="M4" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" ht="13.5" spans="3:13">
       <c r="C5" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="I5" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="M5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="K5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" s="1" customFormat="1" spans="3:12">
+    </row>
+    <row r="6" s="1" customFormat="1" spans="3:13">
       <c r="C6" s="1">
         <v>1001</v>
       </c>
@@ -1317,7 +1331,7 @@
         <v>2</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H6" s="1">
         <v>0</v>
@@ -1326,16 +1340,19 @@
         <v>20</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" s="1" customFormat="1" ht="15" customHeight="1" spans="3:12">
+        <v>17</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" s="1" customFormat="1" ht="15" customHeight="1" spans="3:13">
       <c r="C7" s="1">
         <v>1002</v>
       </c>
@@ -1349,7 +1366,7 @@
         <v>2</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H7" s="1">
         <v>0</v>
@@ -1366,8 +1383,11 @@
       <c r="L7" s="1">
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="3:12">
+      <c r="M7" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="3:13">
       <c r="C8" s="1">
         <v>1003</v>
       </c>
@@ -1398,8 +1418,11 @@
       <c r="L8" s="1">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="3:12">
+      <c r="M8" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="3:13">
       <c r="C9" s="1">
         <v>1004</v>
       </c>
@@ -1430,8 +1453,11 @@
       <c r="L9" s="1">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" spans="3:12">
+      <c r="M9" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="3:13">
       <c r="C10" s="1">
         <v>1005</v>
       </c>
@@ -1462,8 +1488,11 @@
       <c r="L10" s="1">
         <v>30</v>
       </c>
-    </row>
-    <row r="11" spans="3:12">
+      <c r="M10" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="3:13">
       <c r="C11" s="1">
         <v>1006</v>
       </c>
@@ -1477,7 +1506,7 @@
         <v>1</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H11" s="1">
         <v>0</v>
@@ -1494,8 +1523,11 @@
       <c r="L11" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="3:12">
+      <c r="M11" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="3:13">
       <c r="C12" s="1">
         <v>1007</v>
       </c>
@@ -1509,7 +1541,7 @@
         <v>1</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H12" s="1">
         <v>0</v>
@@ -1526,8 +1558,11 @@
       <c r="L12" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="3:12">
+      <c r="M12" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="3:13">
       <c r="C13" s="1">
         <v>1008</v>
       </c>
@@ -1541,7 +1576,7 @@
         <v>3</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H13" s="1">
         <v>0</v>
@@ -1558,8 +1593,11 @@
       <c r="L13" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="3:12">
+      <c r="M13" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="3:13">
       <c r="C14" s="1">
         <v>1009</v>
       </c>
@@ -1573,7 +1611,7 @@
         <v>1</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H14" s="1">
         <v>0</v>
@@ -1590,8 +1628,11 @@
       <c r="L14" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="3:12">
+      <c r="M14" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="3:13">
       <c r="C15" s="1">
         <v>1010</v>
       </c>
@@ -1605,7 +1646,7 @@
         <v>2</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H15" s="1">
         <v>0</v>
@@ -1622,8 +1663,11 @@
       <c r="L15" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="3:12">
+      <c r="M15" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="3:13">
       <c r="C16" s="1">
         <v>1011</v>
       </c>
@@ -1637,7 +1681,7 @@
         <v>3</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H16" s="1">
         <v>0</v>
@@ -1654,8 +1698,11 @@
       <c r="L16" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="3:12">
+      <c r="M16" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="3:13">
       <c r="C17" s="1">
         <v>1012</v>
       </c>
@@ -1669,7 +1716,7 @@
         <v>2</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H17" s="1">
         <v>0</v>
@@ -1686,8 +1733,11 @@
       <c r="L17" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="3:12">
+      <c r="M17" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="3:13">
       <c r="C18" s="1">
         <v>1013</v>
       </c>
@@ -1701,7 +1751,7 @@
         <v>1</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H18" s="1">
         <v>0</v>
@@ -1718,8 +1768,11 @@
       <c r="L18" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="3:12">
+      <c r="M18" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="3:13">
       <c r="C19" s="1">
         <v>1014</v>
       </c>
@@ -1733,7 +1786,7 @@
         <v>2</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H19" s="1">
         <v>0</v>
@@ -1750,8 +1803,11 @@
       <c r="L19" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="20" spans="3:12">
+      <c r="M19" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="3:13">
       <c r="C20" s="1">
         <v>1015</v>
       </c>
@@ -1765,7 +1821,7 @@
         <v>3</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H20" s="1">
         <v>0</v>
@@ -1782,8 +1838,11 @@
       <c r="L20" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="21" spans="3:12">
+      <c r="M20" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="3:13">
       <c r="C21" s="1">
         <v>1016</v>
       </c>
@@ -1797,7 +1856,7 @@
         <v>1</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="H21" s="1">
         <v>0</v>
@@ -1814,8 +1873,11 @@
       <c r="L21" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="22" spans="3:12">
+      <c r="M21" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="3:13">
       <c r="C22" s="1">
         <v>1017</v>
       </c>
@@ -1829,7 +1891,7 @@
         <v>2</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H22" s="1">
         <v>0</v>
@@ -1846,8 +1908,11 @@
       <c r="L22" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="23" spans="3:12">
+      <c r="M22" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="3:13">
       <c r="C23" s="1">
         <v>1018</v>
       </c>
@@ -1861,7 +1926,7 @@
         <v>3</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H23" s="1">
         <v>0</v>
@@ -1878,8 +1943,11 @@
       <c r="L23" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="24" spans="3:12">
+      <c r="M23" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="3:13">
       <c r="C24" s="1">
         <v>1019</v>
       </c>
@@ -1893,7 +1961,7 @@
         <v>1</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H24" s="1">
         <v>0</v>
@@ -1910,8 +1978,11 @@
       <c r="L24" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="3:12">
+      <c r="M24" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="3:13">
       <c r="C25" s="1">
         <v>1020</v>
       </c>
@@ -1925,7 +1996,7 @@
         <v>1</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H25" s="1">
         <v>0</v>
@@ -1942,8 +2013,11 @@
       <c r="L25" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="26" spans="3:12">
+      <c r="M25" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="3:13">
       <c r="C26" s="1">
         <v>1021</v>
       </c>
@@ -1957,7 +2031,7 @@
         <v>2</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="H26" s="1">
         <v>0</v>
@@ -1974,8 +2048,11 @@
       <c r="L26" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="27" spans="3:12">
+      <c r="M26" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="3:13">
       <c r="C27" s="1">
         <v>1022</v>
       </c>
@@ -2006,8 +2083,11 @@
       <c r="L27" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="28" spans="3:12">
+      <c r="M27" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="3:13">
       <c r="C28" s="1">
         <v>1023</v>
       </c>
@@ -2038,8 +2118,11 @@
       <c r="L28" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="29" spans="3:12">
+      <c r="M28" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="3:13">
       <c r="C29" s="1">
         <v>1024</v>
       </c>
@@ -2053,7 +2136,7 @@
         <v>3</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H29" s="1">
         <v>0</v>
@@ -2070,8 +2153,11 @@
       <c r="L29" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="30" spans="3:12">
+      <c r="M29" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="3:13">
       <c r="C30" s="1">
         <v>1025</v>
       </c>
@@ -2085,7 +2171,7 @@
         <v>3</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H30" s="1">
         <v>0</v>
@@ -2102,8 +2188,11 @@
       <c r="L30" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="31" spans="3:12">
+      <c r="M30" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="3:13">
       <c r="C31" s="1">
         <v>1026</v>
       </c>
@@ -2117,7 +2206,7 @@
         <v>1</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H31" s="1">
         <v>0</v>
@@ -2134,8 +2223,11 @@
       <c r="L31" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="32" spans="3:12">
+      <c r="M31" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="3:13">
       <c r="C32" s="1">
         <v>1027</v>
       </c>
@@ -2149,7 +2241,7 @@
         <v>2</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="H32" s="1">
         <v>0</v>
@@ -2166,8 +2258,11 @@
       <c r="L32" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="33" spans="3:12">
+      <c r="M32" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="3:13">
       <c r="C33" s="1">
         <v>1028</v>
       </c>
@@ -2181,7 +2276,7 @@
         <v>1</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H33" s="1">
         <v>0</v>
@@ -2198,8 +2293,11 @@
       <c r="L33" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="34" spans="3:12">
+      <c r="M33" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="3:13">
       <c r="C34" s="1">
         <v>1029</v>
       </c>
@@ -2213,7 +2311,7 @@
         <v>2</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H34" s="1">
         <v>0</v>
@@ -2230,8 +2328,11 @@
       <c r="L34" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="35" spans="3:12">
+      <c r="M34" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="3:13">
       <c r="C35" s="1">
         <v>1030</v>
       </c>
@@ -2245,7 +2346,7 @@
         <v>3</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H35" s="1">
         <v>0</v>
@@ -2262,8 +2363,11 @@
       <c r="L35" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="36" spans="3:12">
+      <c r="M35" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="3:13">
       <c r="C36" s="1">
         <v>1031</v>
       </c>
@@ -2277,7 +2381,7 @@
         <v>1</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="H36" s="1">
         <v>0</v>
@@ -2294,8 +2398,11 @@
       <c r="L36" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="37" spans="3:12">
+      <c r="M36" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="3:13">
       <c r="C37" s="1">
         <v>1032</v>
       </c>
@@ -2309,7 +2416,7 @@
         <v>3</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="H37" s="1">
         <v>0</v>
@@ -2326,8 +2433,11 @@
       <c r="L37" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="38" spans="3:12">
+      <c r="M37" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="3:13">
       <c r="C38" s="1">
         <v>1033</v>
       </c>
@@ -2341,7 +2451,7 @@
         <v>2</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="H38" s="1">
         <v>0</v>
@@ -2358,8 +2468,11 @@
       <c r="L38" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="39" spans="3:12">
+      <c r="M38" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="3:13">
       <c r="C39" s="1">
         <v>1034</v>
       </c>
@@ -2373,7 +2486,7 @@
         <v>3</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="H39" s="1">
         <v>0</v>
@@ -2390,8 +2503,11 @@
       <c r="L39" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="40" spans="3:12">
+      <c r="M39" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" spans="3:13">
       <c r="C40" s="1">
         <v>1035</v>
       </c>
@@ -2405,7 +2521,7 @@
         <v>2</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="H40" s="1">
         <v>0</v>
@@ -2422,8 +2538,11 @@
       <c r="L40" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="41" spans="3:12">
+      <c r="M40" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="3:13">
       <c r="C41" s="1">
         <v>1036</v>
       </c>
@@ -2437,7 +2556,7 @@
         <v>1</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H41" s="1">
         <v>0</v>
@@ -2454,8 +2573,11 @@
       <c r="L41" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="42" spans="3:12">
+      <c r="M41" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="42" spans="3:13">
       <c r="C42" s="1">
         <v>1037</v>
       </c>
@@ -2469,7 +2591,7 @@
         <v>2</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="H42" s="1">
         <v>0</v>
@@ -2486,8 +2608,11 @@
       <c r="L42" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="43" spans="3:12">
+      <c r="M42" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="3:13">
       <c r="C43" s="1">
         <v>1038</v>
       </c>
@@ -2501,7 +2626,7 @@
         <v>1</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="H43" s="1">
         <v>0</v>
@@ -2518,8 +2643,11 @@
       <c r="L43" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="44" spans="3:12">
+      <c r="M43" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="44" spans="3:13">
       <c r="C44" s="1">
         <v>1039</v>
       </c>
@@ -2533,7 +2661,7 @@
         <v>3</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="H44" s="1">
         <v>0</v>
@@ -2550,8 +2678,11 @@
       <c r="L44" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="45" spans="3:12">
+      <c r="M44" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" spans="3:13">
       <c r="C45" s="1">
         <v>1040</v>
       </c>
@@ -2565,7 +2696,7 @@
         <v>2</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H45" s="1">
         <v>0</v>
@@ -2581,6 +2712,9 @@
       </c>
       <c r="L45" s="1">
         <v>5</v>
+      </c>
+      <c r="M45" s="6" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="46" spans="4:4">

</xml_diff>